<commit_message>
[master] updated tutoring act
</commit_message>
<xml_diff>
--- a/guides/tutoring_calendar.xlsx
+++ b/guides/tutoring_calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cappe/Desktop/BWTHW/bwthw/guides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67D0FF7D-60E3-A147-BAB4-6D4C802172D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539C1476-1D8C-8F41-B99E-C8E63B3C772C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4000" yWindow="4220" windowWidth="28800" windowHeight="15980" xr2:uid="{53EB7497-E9FB-664A-B8A3-B594D54FB545}"/>
   </bookViews>
@@ -19,23 +19,12 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">Worksheet!$A$1:$C$13</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Worksheet!$4:$4</definedName>
   </definedNames>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="19">
   <si>
     <t>Day</t>
   </si>
@@ -85,17 +74,20 @@
     <t>TBD</t>
   </si>
   <si>
-    <t>10:30 - 12:30</t>
+    <t>14:30 - 16:30</t>
+  </si>
+  <si>
+    <t>08:30 - 10:30</t>
+  </si>
+  <si>
+    <t>Te+Ue</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
-  </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -106,6 +98,7 @@
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -121,20 +114,25 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <sz val="14"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="14"/>
-      <color indexed="8"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -153,8 +151,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6E0B4"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -177,25 +181,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="14" fontId="5" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -584,7 +601,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="189" zoomScaleNormal="189" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -592,17 +609,17 @@
     <col min="1" max="1" width="13.33203125" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" customWidth="1"/>
     <col min="3" max="3" width="9.83203125" customWidth="1"/>
-    <col min="4" max="4" width="44" customWidth="1"/>
+    <col min="4" max="4" width="51.33203125" customWidth="1"/>
     <col min="5" max="5" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="29" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
     </row>
     <row r="2" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -613,142 +630,142 @@
       <c r="D2" s="4"/>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="5">
-        <v>45722</v>
-      </c>
-      <c r="B5" s="7" t="s">
+        <v>45726</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
-        <v>45729</v>
-      </c>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="6">
+        <v>45733</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="5">
-        <v>45743</v>
-      </c>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="6">
+        <v>45747</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
-        <v>45757</v>
-      </c>
-      <c r="B8" s="7" t="s">
+      <c r="A8" s="6">
+        <v>45761</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="5">
-        <v>45764</v>
-      </c>
-      <c r="B9" s="7" t="s">
+      <c r="A9" s="6">
+        <v>45775</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
-        <v>45785</v>
-      </c>
-      <c r="B10" s="7" t="s">
+      <c r="A10" s="6">
+        <v>45789</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="5">
-        <v>45792</v>
-      </c>
-      <c r="B11" s="7" t="s">
+      <c r="A11" s="6">
+        <v>45796</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
-        <v>45799</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="A12" s="6">
+        <v>45803</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="5">
-        <v>45805</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="A13" s="6">
+        <v>45812</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D13" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -758,6 +775,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" fitToHeight="0" orientation="landscape"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>